<commit_message>
test cases and screenshots
Able to create ticket with missing data.  This did not pass the test case.
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant\School\Classes\CMSC495\Deliverables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stret\Documents\UMGCProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E129071-93E6-45CA-AC62-F8D719C76E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BDE7D1-1297-4837-A0C0-43531CF2037A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{DAC242E4-52C3-4D90-8085-EE16F3248193}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DAC242E4-52C3-4D90-8085-EE16F3248193}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Valid Login By Tech</t>
   </si>
@@ -243,6 +242,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>User able to submit ticket</t>
+  </si>
+  <si>
+    <t>Tech able to submit ticket</t>
+  </si>
+  <si>
+    <t>Tickets were created</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -597,20 +608,20 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.234375" customWidth="1"/>
-    <col min="2" max="2" width="38.76171875" customWidth="1"/>
-    <col min="3" max="3" width="38.3515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.52734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.9375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.64453125" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -630,7 +641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -644,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -658,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -672,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -686,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -699,8 +710,14 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -713,8 +730,14 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -727,8 +750,14 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -748,7 +777,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -768,7 +797,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -788,7 +817,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -808,7 +837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -828,7 +857,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -848,7 +877,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -868,7 +897,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -888,7 +917,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -902,7 +931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -916,7 +945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -930,7 +959,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -944,7 +973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -958,7 +987,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>

</xml_diff>